<commit_message>
Agregue los diagramas, me olvide de hacer push ayer jeje
</commit_message>
<xml_diff>
--- a/JustificacionDeDisenio/Justificaciones-de-Decisiones-para-TP-Anual (1).xlsx
+++ b/JustificacionDeDisenio/Justificaciones-de-Decisiones-para-TP-Anual (1).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
   <si>
     <t>Ambito de decision
 (Objetos / Arquitectura / Persistencia / Otro)</t>
@@ -146,6 +146,60 @@
   </si>
   <si>
     <t>Decidimos que el rescatista tiene usuario, por ende, es mejor que herede de persona y asi tiene un usuario como el duenio</t>
+  </si>
+  <si>
+    <t>Preguntas de la organizacion</t>
+  </si>
+  <si>
+    <t>Hacer un hashmap, que contenga la key de la pregunta junto con su valor de respuesta</t>
+  </si>
+  <si>
+    <t>Hacer un objeto que sea "Pregunta", con un String que seria la pregunta y otro "String" que sea el valor de respuesta</t>
+  </si>
+  <si>
+    <t>Si creabamos el objeto, en el codigo era dificil matchear una pregunta con su equivalente en comodidades del dueño, en cambio teniendo una key es mucho mas sencillo</t>
+  </si>
+  <si>
+    <t>Unificamos el rescate con chapita y sin chapita a una clase rescate</t>
+  </si>
+  <si>
+    <t>Tener dos clases de rescate, una con chapita y otra sin (a modo de strategy)</t>
+  </si>
+  <si>
+    <t>Creemos que es redudante separar entre rescate con chapita y sin chapita, ya que la unica diferencia es que el rescate con chapita conoce que mascota fue encontrada (suponemos que su id), por lo tanto, con poner este atributo nulo, sabemos que tenemos un rescate sin chapita</t>
+  </si>
+  <si>
+    <t>Publicacion</t>
+  </si>
+  <si>
+    <t>Creamos la clase publicacion de la cual heredan los 3 tipos de publicaciones</t>
+  </si>
+  <si>
+    <t>Crear tres clases y repetir los metodos</t>
+  </si>
+  <si>
+    <t>Los 3 tipos de publicaciones usan mismos metodos</t>
+  </si>
+  <si>
+    <t>Adoptante</t>
+  </si>
+  <si>
+    <t>Adoptante hereda de persona</t>
+  </si>
+  <si>
+    <t>Pensamos que el adoptante necesita tener un usuario para realizar las publicaciones correspondientes a la necesidad de adopción, y  además, tiene atributos en comun con persona, por lo tanto implementamos la herencia para evitar la repetición de logica.</t>
+  </si>
+  <si>
+    <t>rescatista-rescate</t>
+  </si>
+  <si>
+    <t>el rescatista conoce a un rescate, y no a la mascota directamente. el rescate conoce a la mascota.</t>
+  </si>
+  <si>
+    <t>que el rescatista conozca a la mascota, y la mascota a su rescate</t>
+  </si>
+  <si>
+    <t>Rescatista no interactua con la mascota, entonces no necesita conocerla, pero si interactua con su rescate, el cual tiene toda la informacion de la misma.</t>
   </si>
 </sst>
 </file>
@@ -170,20 +224,23 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <b/>
       <sz val="11.0"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <color rgb="FFFF0000"/>
       <name val="Docs-Calibri"/>
     </font>
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
     </font>
-    <font>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,6 +251,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF000000"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -223,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -239,17 +308,23 @@
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -482,7 +557,7 @@
     <col customWidth="1" min="2" max="2" width="19.38"/>
     <col customWidth="1" min="3" max="3" width="76.63"/>
     <col customWidth="1" min="4" max="4" width="73.38"/>
-    <col customWidth="1" min="5" max="5" width="44.75"/>
+    <col customWidth="1" min="5" max="5" width="56.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -537,36 +612,36 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="7" t="s">
         <v>21</v>
       </c>
     </row>
@@ -622,19 +697,19 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="8" t="s">
         <v>36</v>
       </c>
     </row>
@@ -673,57 +748,188 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="A12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+      <c r="A13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
+      <c r="A14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
+      <c r="A15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="A16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+    </row>
     <row r="31" ht="15.75" customHeight="1"/>
     <row r="32" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
@@ -1695,7 +1901,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <conditionalFormatting sqref="A2:E17">
+  <conditionalFormatting sqref="A2:E30">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Agrego diagramas y justificaciones
</commit_message>
<xml_diff>
--- a/JustificacionDeDisenio/Justificaciones-de-Decisiones-para-TP-Anual (1).xlsx
+++ b/JustificacionDeDisenio/Justificaciones-de-Decisiones-para-TP-Anual (1).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="81">
   <si>
     <t>Ambito de decision
 (Objetos / Arquitectura / Persistencia / Otro)</t>
@@ -200,6 +200,66 @@
   </si>
   <si>
     <t>Rescatista no interactua con la mascota, entonces no necesita conocerla, pero si interactua con su rescate, el cual tiene toda la informacion de la misma.</t>
+  </si>
+  <si>
+    <t>Persistencia</t>
+  </si>
+  <si>
+    <t>Sistema</t>
+  </si>
+  <si>
+    <t>No persistimos la clase Sistema, solo dejamos las preguntas obligatorias</t>
+  </si>
+  <si>
+    <t>Dejar una clase redundante</t>
+  </si>
+  <si>
+    <t>La clase sistema no tiene nada que persistir, las preguntas obligatorias las ligamos directamente con las organizaciones evitandonos tener una tabla de mas para conectar estas preguntas con las organizaciones.</t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t>Decidimos persistir la clase aunque sean todas claves</t>
+  </si>
+  <si>
+    <t>No persistir</t>
+  </si>
+  <si>
+    <t>tenemos que saber a que organizacion pertenece el adminsitrador, si no mezclamos estas claves no podemos saber esta relacion</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>Guardamos el tipo de usuario como un string</t>
+  </si>
+  <si>
+    <t>Guardarlo como enum</t>
+  </si>
+  <si>
+    <t>Guardamos el tipo de usuario como string, y cuando traemos la informacion de la base de datos ligamos el string con el enum en el constructor de usuario.</t>
+  </si>
+  <si>
+    <t>Hogares de transito</t>
+  </si>
+  <si>
+    <t>Preferimos solo guardar el id de la api del hogar de transito en el rescate</t>
+  </si>
+  <si>
+    <t>Copiar todos los datos y persistirlos</t>
+  </si>
+  <si>
+    <t>No es necesario persistir, hacemos un get en la api y conseguimos los datos</t>
+  </si>
+  <si>
+    <t>Usamos el metodo single table para persistir a la persona y sus hijos</t>
+  </si>
+  <si>
+    <t>Hacer tablas separadas</t>
+  </si>
+  <si>
+    <t>Como persona es una clase abstracta, pensamos en usar este metodo para persistiri al duenio, rescatista, y adoptante. No hay mucho que se le agregue en esta herencia, por eso es mejor meterlo todo en una tabla, gracias al jpa es posible esto.</t>
   </si>
 </sst>
 </file>
@@ -320,11 +380,11 @@
     <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -680,19 +740,19 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="7" t="s">
         <v>32</v>
       </c>
     </row>
@@ -834,101 +894,151 @@
     </row>
     <row r="17">
       <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
     </row>
     <row r="18">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
+      <c r="A18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
+      <c r="A19" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
+      <c r="A20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
+      <c r="A21" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
+      <c r="A22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
     </row>
     <row r="31" ht="15.75" customHeight="1"/>
     <row r="32" ht="15.75" customHeight="1"/>

</xml_diff>